<commit_message>
the latest version 1
</commit_message>
<xml_diff>
--- a/CPR101-GROUP32-V1/module-test-cases-v1.xlsx
+++ b/CPR101-GROUP32-V1/module-test-cases-v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seneca-CPA\CPR101\project\delivery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seneca-CPA\CPR101\project\delivery v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D03F4C-2A8B-4409-8856-3FAE6EA92E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584B8676-6A98-4485-B916-67924B1525D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manipulating" sheetId="3" r:id="rId1"/>
@@ -1504,7 +1504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
   <si>
     <t>Comments</t>
   </si>
@@ -1612,9 +1612,6 @@
     <t>+ Edge case:Verify inputing the two strings containing a total of 79 characters</t>
   </si>
   <si>
-    <t>- Verify inputing  a string containing 80 characters</t>
-  </si>
-  <si>
     <t>"Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^"</t>
   </si>
   <si>
@@ -1652,9 +1649,6 @@
   </si>
   <si>
     <t>Test if program behaves correctly when inputing the two strings containing a total of 79 characters</t>
-  </si>
-  <si>
-    <t>Test if program behaves correctly when inputing a strings beyond the limit of the string's length</t>
   </si>
   <si>
     <t>Test if program behaves correctly when inputing a string that starts with the letter 'q'.</t>
@@ -1697,12 +1691,6 @@
 Word #1 is ',newnewnew'</t>
   </si>
   <si>
-    <t>when using fgets to read user input, if the input exceeds the buffer size (300 characters in this case), only the first 299 characters are read, leaving the remaining characters in the input buffer. If the buffer is not cleared between calls, the next fgets will begin reading from the remaining characters in the buffer, potentially skipping one character, as fgets treats the end of the input as a null terminator.</t>
-  </si>
-  <si>
-    <t>Advice change do-while loop to while loop to avoid this bug. Because do-while loop performs tokenization first and then checks if words is equal to "q". After tokenization, the words variable stores the first tokenized string.</t>
-  </si>
-  <si>
     <t>First string is "q test string"</t>
   </si>
   <si>
@@ -1741,13 +1729,48 @@
 Word #2 is 'string'</t>
   </si>
   <si>
+    <t>' string is equal to ''</t>
+  </si>
+  <si>
     <t>Xiuyan Meng
 2024-11-20</t>
   </si>
   <si>
+    <t>'abc  ' string is greater than 'abc'</t>
+  </si>
+  <si>
+    <t>first string is“abc   ”
+second string is "abc"</t>
+  </si>
+  <si>
+    <t>Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$' string is greater than ''</t>
+  </si>
+  <si>
+    <t>First string is "Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^";
+second string is empty string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display: string is less than 'Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$'
+and prompt use input the first string again
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' string is less than 'Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$'. 
+</t>
+  </si>
+  <si>
+    <t>Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^' string is greater than ''</t>
+  </si>
+  <si>
     <t>"Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$"</t>
   </si>
   <si>
+    <t xml:space="preserve">When input 79 characters, fgets() will not add '\n", then string1[strlen(compare2) - 1] = '\0' replace the last charater with '\0'. It results in the loss of the last character. </t>
+  </si>
+  <si>
+    <t>When input 79 characters, fgets() will not add '\n", then string1[strlen(compare1) - 1] = '\0' replace the last charater with '\0'. It results in the loss of the last character.</t>
+  </si>
+  <si>
     <t xml:space="preserve">When input 79 characters, fgets() will not add '\n", then string1[strlen(string2) - 1] = '\0' replace the last charater with '\0'. It results in the loss of the last character. </t>
   </si>
   <si>
@@ -1761,6 +1784,60 @@
   </si>
   <si>
     <t>One string is "Test string that have 80 characters Test string", another is "that have 80 characters,’’%^&amp;*$#"</t>
+  </si>
+  <si>
+    <t>"Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^#beyond"</t>
+  </si>
+  <si>
+    <t>Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$' string is greater than '#beyond'</t>
+  </si>
+  <si>
+    <t>This bug is caused by how fgets() works. It is recommended to add code to clear the buffer and provide a prompt.</t>
+  </si>
+  <si>
+    <t>prompt invalid input OR
+'Test string that have 80 characters Test stringEND' string is greater than ' that have 80 characters,&amp;$#@%$^#beyond'</t>
+  </si>
+  <si>
+    <t>Test string that have 80 characters Test stringEND' string is greater than ' that have 80 characters,&amp;$#@%$^#beyond'</t>
+  </si>
+  <si>
+    <t>prompt invalid input OR
+'Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^#beyond' is greater than ''</t>
+  </si>
+  <si>
+    <t>'q v' string is greater than 'q ffg'</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputing  two same string</t>
+  </si>
+  <si>
+    <t>Two string both are "abc"</t>
+  </si>
+  <si>
+    <t>'abc' string is equal to 'abc'</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputing  the first string less than the sencond string</t>
+  </si>
+  <si>
+    <t>+Verify inputing inputing  the first string less than the sencond string</t>
+  </si>
+  <si>
+    <t>+Verify inputing two same string.</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputing a string "q" as the first string</t>
+  </si>
+  <si>
+    <t>+Verify inputing a string "q" as first string.</t>
+  </si>
+  <si>
+    <t>First string is "aba",
+second string is "abd"</t>
+  </si>
+  <si>
+    <t>'aba' string is less than 'abd'</t>
   </si>
   <si>
     <t>+Verify inputing a string containing multiple consecutive spaces.</t>
@@ -1779,19 +1856,116 @@
     <t>+ Edge case:Verify inputing  a string containing 298 characters</t>
   </si>
   <si>
-    <t>"Test,string,that,have,80,characters Test,string,that,have,80,characters &amp;$#@%$^,Test,string,that,have,80,characters Test,string,that,have,80,characters,&amp;$#@%$^Test,string,that,have,80,characters,Test,string that,have,80,characters,&amp;$#@%$^,Test,string,that have,80,characters,Test,string,that,have,8"</t>
-  </si>
-  <si>
-    <t>Word #1 is 'Test,string,that,have,80,characters'
+    <t>Test if program behaves correctly when inputting a string containing 298 characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> " "found at 0 position</t>
+  </si>
+  <si>
+    <t>""found at 0 position</t>
+  </si>
+  <si>
+    <t>+Verify multiple substrings in string</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when multiple substrings in string</t>
+  </si>
+  <si>
+    <t>string is two spaces
+substring is one space</t>
+  </si>
+  <si>
+    <t>string is "hfgabcdefgabc"
+substring is "abc"</t>
+  </si>
+  <si>
+    <t>"abc" found at 3 position</t>
+  </si>
+  <si>
+    <t>string is "Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^";
+substring is "string"</t>
+  </si>
+  <si>
+    <t>"string" found at 5 position</t>
+  </si>
+  <si>
+    <t>" found at 0 position</t>
+  </si>
+  <si>
+    <t>string is "Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$";
+substring is ",&amp;"</t>
+  </si>
+  <si>
+    <t>",&amp;" found at 71 position</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputting a string containing 78 characters</t>
+  </si>
+  <si>
+    <t>+ Verify inputing  the first string containing 78 characters</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>First string is "q v"; second string is"q "</t>
+  </si>
+  <si>
+    <t>'q' found at 0 position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When input 79 characters, fgets() function get 79 characters and leave "\0" in the input buffer results in the user being unable to input the substring. </t>
+  </si>
+  <si>
+    <t>- Verify inputing  a string containing more than 80 characters</t>
+  </si>
+  <si>
+    <t>One string is "Test string that have 80 characters Test stringEND",
+ another is "that have 80 characters,&amp;$#@%$^#beyond"</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputing a substring beyond the limit of the string's length</t>
+  </si>
+  <si>
+    <t>Test if program behaves correctly when inputing a string beyond the limit of the string's length</t>
+  </si>
+  <si>
+    <t>Not found and the user being unable to input the string when user want to try again.</t>
+  </si>
+  <si>
+    <t>- Verify inputing  a substring containing more than 80 characters</t>
+  </si>
+  <si>
+    <t>string is "Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^#beyond"</t>
+  </si>
+  <si>
+    <t>string is "test"
+substring is "Test string that have 80 characters Test string that have 80 characters,&amp;$#@%$^#beyond"</t>
+  </si>
+  <si>
+    <t>Advice change do-while loop to avoid this bug. Because do-while loop performs tokenization first and then checks if words is equal to "q". After tokenization, the words variable stores the first tokenized string.</t>
+  </si>
+  <si>
+    <t>Xiuyan Meng
+2024-11-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word #1 is 'Test,string,that,have,80,characters'
 Word #2 is 'Test,string,that,have,80,characters,'
 Word #3 is '&amp;$#@%$^,Test,string,that,have,80,characters,'
 Word #4 is 'Test,string,that,have,80,characters,&amp;$#@%$^Test,string,that,have,80,characters,Test,string,that,have,80,characters,&amp;$#@%$^,Test,string,that,'
 Word #5 is 'have,80,characters,Test,string,that,hav'
 Type a few words separated by space (q - to quit):
-Word #1 is ',8'</t>
-  </si>
-  <si>
-    <t>Test if program behaves correctly when inputting a string containing 298 characters</t>
+</t>
+  </si>
+  <si>
+    <t>"Test,string,that,have,80,characters Test,string,that,have,80,characters &amp;$#@%$^,Test,string,that,have,80,characters Test,string,that,have,80,characters,&amp;$#@%$^Test,string,that,have,80,characters,Test,string that,have,80,characters,&amp;$#@%$^,Test,string,that have,80,characters,Test,string,that,have"</t>
+  </si>
+  <si>
+    <t>when using fgets to read user input, if the input exceeds the buffer size (300 characters in this case), fgets will get 298 characters and \n, then add '\0' at the end. leaving the remaining characters in the input buffer. If the buffer is not cleared between calls, the next fgets will begin reading from the remaining characters in the buffer, potentially skipping one character, as fgets treats the end of the input as a null terminator.</t>
+  </si>
+  <si>
+    <t>fgets() function get  up to  79 characters and leave remaining characters in the input buffer results in the user being unable to input the substring.</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2249,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2212,6 +2386,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2555,10 +2732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2568,7 +2745,7 @@
     <col min="3" max="3" width="29.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2579,23 +2756,23 @@
       <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="49" t="str">
+      <c r="C1" s="50" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
       <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
@@ -2628,10 +2805,10 @@
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>16</v>
@@ -2647,7 +2824,7 @@
     </row>
     <row r="5" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>15</v>
@@ -2666,74 +2843,74 @@
     </row>
     <row r="6" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>22</v>
@@ -2742,50 +2919,50 @@
         <v>23</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>33</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="21" t="s">
@@ -2795,16 +2972,16 @@
     </row>
     <row r="12" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="21" t="s">
@@ -2857,18 +3034,18 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -2894,83 +3071,202 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="F20" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+      <c r="F21" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="E26" s="19"/>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="F26" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="E27" s="19"/>
-      <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
+      <c r="F27" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
+      <c r="F28" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="21"/>
+      <c r="F29" s="21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
@@ -2985,13 +3281,13 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="12" t="s">
         <v>5</v>
       </c>
@@ -3022,59 +3318,188 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
+    <row r="34" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
+      <c r="F34" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>101</v>
+      </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
+      <c r="F35" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>107</v>
+      </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
+      <c r="F36" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="21"/>
+      <c r="F38" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="19"/>
+      <c r="F41" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="19"/>
+      <c r="F42" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="26"/>
+      <c r="B43" s="27"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3101,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED336A4-B639-43A9-ABB0-9651F7DECFAE}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="A15:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3110,9 +3535,9 @@
     <col min="1" max="1" width="14.28515625" style="30" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="46.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" style="39" customWidth="1"/>
-    <col min="6" max="6" width="29" style="44" customWidth="1"/>
+    <col min="6" max="6" width="17" style="44" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="30"/>
   </cols>
@@ -3122,25 +3547,25 @@
         <v>3</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="51" t="str">
+        <v>55</v>
+      </c>
+      <c r="C1" s="52" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As tokenizing_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="31" t="s">
         <v>5</v>
       </c>
@@ -3173,16 +3598,16 @@
     </row>
     <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6" t="s">
@@ -3193,16 +3618,16 @@
     </row>
     <row r="5" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
@@ -3210,18 +3635,18 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="315" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="270" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="6" t="s">
@@ -3230,42 +3655,42 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="38" t="s">
         <v>60</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>64</v>
       </c>
       <c r="E8" s="45"/>
       <c r="F8" s="6" t="s">
@@ -3274,41 +3699,41 @@
       <c r="G8" s="9"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
@@ -3335,18 +3760,18 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="31" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3480,18 +3905,18 @@
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="32" t="s">
-        <v>14</v>
+      <c r="G29" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3517,55 +3942,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="43"/>
+    <row r="31" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="8"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="43"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="8"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43"/>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="38"/>
       <c r="E33" s="8"/>
       <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="8"/>
       <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="8"/>
       <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
-      <c r="B36" s="43"/>
-      <c r="E36" s="8"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
-      <c r="B37" s="43"/>
-      <c r="E37" s="8"/>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="42"/>
       <c r="B38" s="43"/>
       <c r="E38" s="8"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="42"/>
       <c r="B39" s="43"/>
       <c r="E39" s="8"/>

</xml_diff>